<commit_message>
Reviewed in full the main algorithm for testing with N2. Happy with the results. Now working on the algorithm to plot as the experiment advances
</commit_message>
<xml_diff>
--- a/nitrogen_experiments/N2_test_summary.xlsx
+++ b/nitrogen_experiments/N2_test_summary.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16230" windowHeight="11730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16230" windowHeight="11730" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="valid_experiments" sheetId="1" r:id="rId1"/>
+    <sheet name="Trials" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,9 +25,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="11">
   <si>
     <t>Test_number</t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>timber</t>
+  </si>
+  <si>
+    <t>pmma</t>
+  </si>
+  <si>
+    <t>pmma_clear</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>pa6</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>thickness_mm</t>
+  </si>
+  <si>
+    <t>constant_mlr_nominal_gm-2s-1</t>
+  </si>
+  <si>
+    <t>N2_flow_lpm</t>
   </si>
 </sst>
 </file>
@@ -344,17 +375,650 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2.5</v>
+      </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2.5</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>7.5</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>7.5</v>
+      </c>
+      <c r="F7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>2.5</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>2.5</v>
+      </c>
+      <c r="F11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>7.5</v>
+      </c>
+      <c r="F14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>7.5</v>
+      </c>
+      <c r="F15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>2.5</v>
+      </c>
+      <c r="F18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>2.5</v>
+      </c>
+      <c r="F19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>7.5</v>
+      </c>
+      <c r="F22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>7.5</v>
+      </c>
+      <c r="F23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>10</v>
+      </c>
+      <c r="F24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <v>2.5</v>
+      </c>
+      <c r="F26">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27">
+        <v>2.5</v>
+      </c>
+      <c r="F27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30">
+        <v>7.5</v>
+      </c>
+      <c r="F30">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31">
+        <v>7.5</v>
+      </c>
+      <c r="F31">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32">
+        <v>10</v>
+      </c>
+      <c r="F32">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2.5</v>
+      </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>7.5</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>2.5</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>7.5</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished nitrogen experiments, for now!
</commit_message>
<xml_diff>
--- a/nitrogen_experiments/N2_test_summary.xlsx
+++ b/nitrogen_experiments/N2_test_summary.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="51">
   <si>
     <t>Test_number</t>
   </si>
@@ -156,7 +156,28 @@
     <t>Repeat of 008. Some oscillations, but overall, much more stable.</t>
   </si>
   <si>
-    <t>First experiment with clear PMMA.</t>
+    <t>First experiment with clear PMMA. Very noisy, driven in part by the fact that the PID was activated almost from time = 0. I wonder if using a lower inlet flow will improve the behaivour. Tape around insulation loosened, and so it is possible there was some interference with the load cell. Aluminium block at the end of the test was very hot. Probably, at these wavelengths, transmissivity of the clear pmma is high.</t>
+  </si>
+  <si>
+    <t>Reduced the N2 inlet for for this experiment to see how much of an effect that has on the mass readings and the performance of the PID controller. Very good results, much more stable and lack of initial noise allowed for the full growth in the HF curve.</t>
+  </si>
+  <si>
+    <t>Repeat of 011 but lower N2 flow.</t>
+  </si>
+  <si>
+    <t>Following previous results, I will now do one at 50 lpm and one at 20 lpm. Quie noisy.</t>
+  </si>
+  <si>
+    <t>First test with PA6. Seemed ok. Bit noisy as always with this flow rate.</t>
+  </si>
+  <si>
+    <t>Repeat of 013. I should have used a flow of 20, but I made a mistake when setting the flow and ended up using 50. Ok behaviour.</t>
+  </si>
+  <si>
+    <t>Went OK. A bit noisy the signal, as always when 50 is used.</t>
+  </si>
+  <si>
+    <t>Gases from PA6 seem heavier, more dense. Because the extraction flow is lower, it actually becomes difficult to see the surface sample (it seems that the camera has the same problem).</t>
   </si>
 </sst>
 </file>
@@ -514,9 +535,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -529,7 +550,7 @@
     <col min="6" max="6" width="29.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29" style="10" customWidth="1"/>
+    <col min="9" max="9" width="37.28515625" style="9" customWidth="1"/>
     <col min="10" max="11" width="20" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="6"/>
   </cols>
@@ -1064,7 +1085,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="165" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>9</v>
       </c>
@@ -1089,14 +1110,17 @@
       <c r="H13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="9" t="s">
         <v>43</v>
       </c>
       <c r="J13" s="6">
         <v>0</v>
       </c>
+      <c r="K13" s="6">
+        <v>60</v>
+      </c>
       <c r="L13" s="6">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="M13" s="6">
         <v>0.04</v>
@@ -1105,7 +1129,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>10</v>
       </c>
@@ -1125,16 +1149,32 @@
         <v>2</v>
       </c>
       <c r="G14" s="6">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="I14" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="J14" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="6">
+        <f>2*60+12</f>
+        <v>132</v>
+      </c>
+      <c r="L14" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="M14" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="N14" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>11</v>
       </c>
@@ -1159,8 +1199,23 @@
       <c r="H15" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="I15" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="J15" s="6">
         <v>0</v>
+      </c>
+      <c r="K15" s="6">
+        <v>70</v>
+      </c>
+      <c r="L15" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="M15" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="N15" s="6">
+        <v>0.2</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1183,22 +1238,40 @@
         <v>4</v>
       </c>
       <c r="G16" s="6">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="I16" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="J16" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="6">
+        <v>20</v>
+      </c>
+      <c r="L16" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="M16" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="N16" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>13</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="C17" s="7">
+        <v>44179</v>
+      </c>
       <c r="D17" s="6">
         <v>20</v>
       </c>
@@ -1214,17 +1287,35 @@
       <c r="H17" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="I17" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="J17" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="6">
+        <v>66</v>
+      </c>
+      <c r="L17" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="M17" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="N17" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>14</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="C18" s="7">
+        <v>44179</v>
+      </c>
       <c r="D18" s="6">
         <v>20</v>
       </c>
@@ -1240,17 +1331,36 @@
       <c r="H18" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="I18" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="J18" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="6">
+        <f>60+19</f>
+        <v>79</v>
+      </c>
+      <c r="L18" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="M18" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="N18" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>15</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="C19" s="7">
+        <v>44179</v>
+      </c>
       <c r="D19" s="6">
         <v>20</v>
       </c>
@@ -1266,17 +1376,36 @@
       <c r="H19" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="I19" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="J19" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="6">
+        <f>60+35</f>
+        <v>95</v>
+      </c>
+      <c r="L19" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="M19" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="N19" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>16</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="C20" s="7">
+        <v>44179</v>
+      </c>
       <c r="D20" s="6">
         <v>20</v>
       </c>
@@ -1287,13 +1416,28 @@
         <v>4</v>
       </c>
       <c r="G20" s="6">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="I20" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="J20" s="6">
         <v>0</v>
+      </c>
+      <c r="K20" s="6">
+        <v>83</v>
+      </c>
+      <c r="L20" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="M20" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="N20" s="6">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>